<commit_message>
add rows on demand
</commit_message>
<xml_diff>
--- a/testdata/Parse German Date.xlsx
+++ b/testdata/Parse German Date.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/axelhowind/Projects/meja/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B2A9408-4C0D-5E45-8498-E2581EE8EE76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03730A8B-68F8-C142-B56D-D8A97CA3BAAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6720" yWindow="4100" windowWidth="27840" windowHeight="16740" xr2:uid="{9B4993B0-F47A-F34D-BD65-692D2AEC7FA9}"/>
   </bookViews>
@@ -423,14 +423,14 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
-        <f>("1." &amp; A3 &amp; "." &amp; A4)*1</f>
+        <f>("1. " &amp; A3 &amp; " " &amp; A4)*1</f>
         <v>45658</v>
       </c>
       <c r="B1" t="s">

</xml_diff>